<commit_message>
adding the grades and fixing a bug in grade.py
</commit_message>
<xml_diff>
--- a/CA04/grades.xlsx
+++ b/CA04/grades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amirmy/Desktop/4034_2/Advanced Programing_TA/HWs/CA04/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C01499DC-FED7-5448-B5A1-0C5A22EB04BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1E2D679-599B-8C48-8373-2C0E8E17F71E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{5279A396-C080-7743-B686-4EC8ED3EC883}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="39">
   <si>
     <t>Q1</t>
   </si>
@@ -409,24 +409,6 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -455,167 +437,33 @@
     <xf numFmtId="0" fontId="12" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFAEAAAA"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6E0B4"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFAEAAAA"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6E0B4"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFAEAAAA"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6E0B4"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFAEAAAA"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6E0B4"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFAEAAAA"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6E0B4"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFAEAAAA"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6E0B4"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFAEAAAA"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6E0B4"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6E0B4"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6E0B4"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6E0B4"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6E0B4"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6E0B4"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6E0B4"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
@@ -941,8 +789,8 @@
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K11" sqref="K11"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -954,41 +802,41 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="B1" s="1"/>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="9"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="11" t="s">
+      <c r="D1" s="21"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="12"/>
-      <c r="H1" s="13"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="25"/>
       <c r="I1" s="1"/>
     </row>
     <row r="2" spans="1:10" ht="19">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="D2" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="E2" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="F2" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="G2" s="23" t="s">
+      <c r="G2" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="H2" s="23" t="s">
+      <c r="H2" s="17" t="s">
         <v>38</v>
       </c>
       <c r="I2" s="6" t="s">
@@ -996,14 +844,14 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="19">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="14">
+      <c r="B3" s="8">
         <v>810803092</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>4</v>
+      <c r="C3" s="3">
+        <v>40</v>
       </c>
       <c r="D3" s="3">
         <v>40</v>
@@ -1025,14 +873,14 @@
       </c>
     </row>
     <row r="4" spans="1:10" ht="19">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="14">
+      <c r="B4" s="8">
         <v>810803074</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>4</v>
+      <c r="C4" s="3">
+        <v>40</v>
       </c>
       <c r="D4" s="3">
         <v>40</v>
@@ -1054,10 +902,10 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="19">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="14">
+      <c r="B5" s="8">
         <v>810803081</v>
       </c>
       <c r="C5" s="3">
@@ -1083,14 +931,14 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="19">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="15">
+      <c r="B6" s="9">
         <v>810802068</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>4</v>
+      <c r="C6" s="3">
+        <v>40</v>
       </c>
       <c r="D6" s="3">
         <v>40</v>
@@ -1098,8 +946,8 @@
       <c r="E6" s="2">
         <v>20</v>
       </c>
-      <c r="F6" s="4" t="s">
-        <v>4</v>
+      <c r="F6" s="4">
+        <v>40</v>
       </c>
       <c r="G6" s="5">
         <v>40</v>
@@ -1112,14 +960,14 @@
       </c>
     </row>
     <row r="7" spans="1:10" ht="19">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="15">
+      <c r="B7" s="9">
         <v>810802083</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>4</v>
+      <c r="C7" s="3">
+        <v>40</v>
       </c>
       <c r="D7" s="3">
         <v>20</v>
@@ -1127,8 +975,8 @@
       <c r="E7" s="2">
         <v>20</v>
       </c>
-      <c r="F7" s="4" t="s">
-        <v>4</v>
+      <c r="F7" s="4">
+        <v>40</v>
       </c>
       <c r="G7" s="5">
         <v>20</v>
@@ -1141,14 +989,14 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="19">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="16">
+      <c r="B8" s="10">
         <v>810803075</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>4</v>
+      <c r="C8" s="3">
+        <v>40</v>
       </c>
       <c r="D8" s="3">
         <v>40</v>
@@ -1156,8 +1004,8 @@
       <c r="E8" s="2">
         <v>20</v>
       </c>
-      <c r="F8" s="4" t="s">
-        <v>4</v>
+      <c r="F8" s="4">
+        <v>40</v>
       </c>
       <c r="G8" s="5">
         <v>40</v>
@@ -1170,14 +1018,14 @@
       </c>
     </row>
     <row r="9" spans="1:10" ht="19">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="15">
+      <c r="B9" s="9">
         <v>810801074</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>4</v>
+      <c r="C9" s="3">
+        <v>40</v>
       </c>
       <c r="D9" s="3">
         <v>40</v>
@@ -1185,8 +1033,8 @@
       <c r="E9" s="2">
         <v>20</v>
       </c>
-      <c r="F9" s="4" t="s">
-        <v>4</v>
+      <c r="F9" s="4">
+        <v>40</v>
       </c>
       <c r="G9" s="5">
         <v>40</v>
@@ -1199,14 +1047,14 @@
       </c>
     </row>
     <row r="10" spans="1:10" ht="19">
-      <c r="A10" s="18" t="s">
+      <c r="A10" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="15">
+      <c r="B10" s="9">
         <v>810803069</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>4</v>
+      <c r="C10" s="3">
+        <v>40</v>
       </c>
       <c r="D10" s="3">
         <v>40</v>
@@ -1214,8 +1062,8 @@
       <c r="E10" s="2">
         <v>15</v>
       </c>
-      <c r="F10" s="4" t="s">
-        <v>4</v>
+      <c r="F10" s="4">
+        <v>40</v>
       </c>
       <c r="G10" s="5">
         <v>40</v>
@@ -1228,14 +1076,14 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="19">
-      <c r="A11" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="15">
+      <c r="A11" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="9">
         <v>810802089</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>4</v>
+      <c r="C11" s="3">
+        <v>40</v>
       </c>
       <c r="D11" s="3">
         <v>30</v>
@@ -1243,8 +1091,8 @@
       <c r="E11" s="2">
         <v>10</v>
       </c>
-      <c r="F11" s="4" t="s">
-        <v>4</v>
+      <c r="F11" s="4">
+        <v>40</v>
       </c>
       <c r="G11" s="5">
         <v>30</v>
@@ -1257,14 +1105,14 @@
       </c>
     </row>
     <row r="12" spans="1:10" ht="19">
-      <c r="A12" s="18" t="s">
+      <c r="A12" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="15">
+      <c r="B12" s="9">
         <v>810800006</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>4</v>
+      <c r="C12" s="3">
+        <v>40</v>
       </c>
       <c r="D12" s="3">
         <v>40</v>
@@ -1272,8 +1120,8 @@
       <c r="E12" s="2">
         <v>20</v>
       </c>
-      <c r="F12" s="4" t="s">
-        <v>4</v>
+      <c r="F12" s="4">
+        <v>40</v>
       </c>
       <c r="G12" s="5">
         <v>40</v>
@@ -1286,14 +1134,14 @@
       </c>
     </row>
     <row r="13" spans="1:10" ht="19">
-      <c r="A13" s="18" t="s">
+      <c r="A13" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="15">
+      <c r="B13" s="9">
         <v>810801064</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>4</v>
+      <c r="C13" s="3">
+        <v>40</v>
       </c>
       <c r="D13" s="3">
         <v>40</v>
@@ -1301,8 +1149,8 @@
       <c r="E13" s="2">
         <v>20</v>
       </c>
-      <c r="F13" s="4" t="s">
-        <v>4</v>
+      <c r="F13" s="4">
+        <v>40</v>
       </c>
       <c r="G13" s="5">
         <v>40</v>
@@ -1315,14 +1163,14 @@
       </c>
     </row>
     <row r="14" spans="1:10" ht="19">
-      <c r="A14" s="18" t="s">
+      <c r="A14" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="15">
+      <c r="B14" s="9">
         <v>810801065</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>4</v>
+      <c r="C14" s="3">
+        <v>40</v>
       </c>
       <c r="D14" s="3">
         <v>30</v>
@@ -1330,8 +1178,8 @@
       <c r="E14" s="2">
         <v>10</v>
       </c>
-      <c r="F14" s="4" t="s">
-        <v>4</v>
+      <c r="F14" s="4">
+        <v>40</v>
       </c>
       <c r="G14" s="5">
         <v>30</v>
@@ -1344,14 +1192,14 @@
       </c>
     </row>
     <row r="15" spans="1:10" ht="19">
-      <c r="A15" s="18" t="s">
+      <c r="A15" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="15">
+      <c r="B15" s="9">
         <v>810802082</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>4</v>
+      <c r="C15" s="3">
+        <v>40</v>
       </c>
       <c r="D15" s="3">
         <v>30</v>
@@ -1359,8 +1207,8 @@
       <c r="E15" s="2">
         <v>10</v>
       </c>
-      <c r="F15" s="4" t="s">
-        <v>4</v>
+      <c r="F15" s="4">
+        <v>40</v>
       </c>
       <c r="G15" s="5">
         <v>30</v>
@@ -1371,17 +1219,17 @@
       <c r="I15" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="J15" s="19"/>
+      <c r="J15" s="13"/>
     </row>
     <row r="16" spans="1:10" ht="19">
-      <c r="A16" s="18" t="s">
+      <c r="A16" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="15">
+      <c r="B16" s="9">
         <v>810803098</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>4</v>
+      <c r="C16" s="3">
+        <v>40</v>
       </c>
       <c r="D16" s="3">
         <v>40</v>
@@ -1389,8 +1237,8 @@
       <c r="E16" s="2">
         <v>20</v>
       </c>
-      <c r="F16" s="4" t="s">
-        <v>4</v>
+      <c r="F16" s="4">
+        <v>40</v>
       </c>
       <c r="G16" s="5">
         <v>40</v>
@@ -1403,14 +1251,14 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="19">
-      <c r="A17" s="18" t="s">
+      <c r="A17" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="15">
+      <c r="B17" s="9">
         <v>810801085</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>4</v>
+      <c r="C17" s="3">
+        <v>40</v>
       </c>
       <c r="D17" s="3">
         <v>40</v>
@@ -1418,8 +1266,8 @@
       <c r="E17" s="2">
         <v>20</v>
       </c>
-      <c r="F17" s="4" t="s">
-        <v>4</v>
+      <c r="F17" s="4">
+        <v>40</v>
       </c>
       <c r="G17" s="5">
         <v>40</v>
@@ -1432,14 +1280,14 @@
       </c>
     </row>
     <row r="18" spans="1:9" ht="19">
-      <c r="A18" s="18" t="s">
+      <c r="A18" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="15">
+      <c r="B18" s="9">
         <v>810802076</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>4</v>
+      <c r="C18" s="3">
+        <v>40</v>
       </c>
       <c r="D18" s="3">
         <v>40</v>
@@ -1447,8 +1295,8 @@
       <c r="E18" s="2">
         <v>20</v>
       </c>
-      <c r="F18" s="4" t="s">
-        <v>4</v>
+      <c r="F18" s="4">
+        <v>40</v>
       </c>
       <c r="G18" s="5">
         <v>40</v>
@@ -1461,14 +1309,14 @@
       </c>
     </row>
     <row r="19" spans="1:9" ht="19">
-      <c r="A19" s="18" t="s">
+      <c r="A19" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B19" s="15">
+      <c r="B19" s="9">
         <v>810800025</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>4</v>
+      <c r="C19" s="3">
+        <v>40</v>
       </c>
       <c r="D19" s="3">
         <v>40</v>
@@ -1476,8 +1324,8 @@
       <c r="E19" s="2">
         <v>20</v>
       </c>
-      <c r="F19" s="4" t="s">
-        <v>4</v>
+      <c r="F19" s="4">
+        <v>40</v>
       </c>
       <c r="G19" s="5">
         <v>40</v>
@@ -1490,14 +1338,14 @@
       </c>
     </row>
     <row r="20" spans="1:9" ht="19">
-      <c r="A20" s="18" t="s">
+      <c r="A20" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="15">
+      <c r="B20" s="9">
         <v>810802064</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>4</v>
+      <c r="C20" s="3">
+        <v>40</v>
       </c>
       <c r="D20" s="3">
         <v>40</v>
@@ -1505,8 +1353,8 @@
       <c r="E20" s="2">
         <v>5</v>
       </c>
-      <c r="F20" s="4" t="s">
-        <v>4</v>
+      <c r="F20" s="4">
+        <v>40</v>
       </c>
       <c r="G20" s="5">
         <v>40</v>
@@ -1519,14 +1367,14 @@
       </c>
     </row>
     <row r="21" spans="1:9" ht="19">
-      <c r="A21" s="18" t="s">
+      <c r="A21" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="15">
+      <c r="B21" s="9">
         <v>810101556</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>4</v>
+      <c r="C21" s="3">
+        <v>40</v>
       </c>
       <c r="D21" s="3">
         <v>40</v>
@@ -1534,8 +1382,8 @@
       <c r="E21" s="2">
         <v>10</v>
       </c>
-      <c r="F21" s="4" t="s">
-        <v>4</v>
+      <c r="F21" s="4">
+        <v>40</v>
       </c>
       <c r="G21" s="5">
         <v>40</v>
@@ -1548,10 +1396,10 @@
       </c>
     </row>
     <row r="22" spans="1:9" ht="19">
-      <c r="A22" s="20" t="s">
+      <c r="A22" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="15">
+      <c r="B22" s="9">
         <v>810801071</v>
       </c>
       <c r="C22" s="2" t="s">
@@ -1577,10 +1425,10 @@
       </c>
     </row>
     <row r="23" spans="1:9" ht="19">
-      <c r="A23" s="20" t="s">
+      <c r="A23" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="B23" s="15">
+      <c r="B23" s="9">
         <v>810802073</v>
       </c>
       <c r="C23" s="2" t="s">
@@ -1606,10 +1454,10 @@
       </c>
     </row>
     <row r="24" spans="1:9" ht="19">
-      <c r="A24" s="17" t="s">
+      <c r="A24" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B24" s="15">
+      <c r="B24" s="9">
         <v>810801083</v>
       </c>
       <c r="C24" s="2" t="s">
@@ -1635,10 +1483,10 @@
       </c>
     </row>
     <row r="25" spans="1:9" ht="19">
-      <c r="A25" s="17" t="s">
+      <c r="A25" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B25" s="15">
+      <c r="B25" s="9">
         <v>810801057</v>
       </c>
       <c r="C25" s="2" t="s">
@@ -1664,10 +1512,10 @@
       </c>
     </row>
     <row r="26" spans="1:9" ht="19">
-      <c r="A26" s="17" t="s">
+      <c r="A26" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="B26" s="15">
+      <c r="B26" s="9">
         <v>810101589</v>
       </c>
       <c r="C26" s="2" t="s">
@@ -1693,10 +1541,10 @@
       </c>
     </row>
     <row r="27" spans="1:9" ht="19">
-      <c r="A27" s="17" t="s">
+      <c r="A27" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="B27" s="15">
+      <c r="B27" s="9">
         <v>810800003</v>
       </c>
       <c r="C27" s="2" t="s">
@@ -1722,10 +1570,10 @@
       </c>
     </row>
     <row r="28" spans="1:9" ht="19">
-      <c r="A28" s="17" t="s">
+      <c r="A28" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="B28" s="15">
+      <c r="B28" s="9">
         <v>810802063</v>
       </c>
       <c r="C28" s="2" t="s">
@@ -1751,10 +1599,10 @@
       </c>
     </row>
     <row r="29" spans="1:9" ht="19">
-      <c r="A29" s="17" t="s">
+      <c r="A29" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B29" s="15">
+      <c r="B29" s="9">
         <v>810802070</v>
       </c>
       <c r="C29" s="2" t="s">
@@ -1780,10 +1628,10 @@
       </c>
     </row>
     <row r="30" spans="1:9" ht="19">
-      <c r="A30" s="17" t="s">
+      <c r="A30" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="B30" s="15">
+      <c r="B30" s="9">
         <v>810802077</v>
       </c>
       <c r="C30" s="2" t="s">
@@ -1809,10 +1657,10 @@
       </c>
     </row>
     <row r="31" spans="1:9" ht="19">
-      <c r="A31" s="17" t="s">
+      <c r="A31" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="B31" s="15">
+      <c r="B31" s="9">
         <v>810899054</v>
       </c>
       <c r="C31" s="2" t="s">
@@ -1838,10 +1686,10 @@
       </c>
     </row>
     <row r="32" spans="1:9" ht="19">
-      <c r="A32" s="17" t="s">
+      <c r="A32" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="B32" s="15">
+      <c r="B32" s="9">
         <v>810899066</v>
       </c>
       <c r="C32" s="2" t="s">
@@ -1868,8 +1716,8 @@
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:I32">
-    <sortCondition sortBy="cellColor" ref="A3:A32" dxfId="3"/>
-    <sortCondition descending="1" sortBy="cellColor" ref="A3:A32" dxfId="2"/>
+    <sortCondition sortBy="cellColor" ref="A3:A32" dxfId="1"/>
+    <sortCondition descending="1" sortBy="cellColor" ref="A3:A32" dxfId="0"/>
   </sortState>
   <mergeCells count="2">
     <mergeCell ref="C1:E1"/>

</xml_diff>